<commit_message>
added code and data. no graph yet
</commit_message>
<xml_diff>
--- a/Experiment 1/Trace Files/LatencyGraph.xlsx
+++ b/Experiment 1/Trace Files/LatencyGraph.xlsx
@@ -602,11 +602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="507593824"/>
-        <c:axId val="507588384"/>
+        <c:axId val="210620352"/>
+        <c:axId val="420602560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="507593824"/>
+        <c:axId val="210620352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507588384"/>
+        <c:crossAx val="420602560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,7 +713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="507588384"/>
+        <c:axId val="420602560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="28"/>
@@ -755,7 +755,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Latency (ms)</a:t>
+                  <a:t>Round Trip Time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -821,7 +821,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="507593824"/>
+        <c:crossAx val="210620352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>

<commit_message>
experiment 1 throughput/latency fix
</commit_message>
<xml_diff>
--- a/Experiment 1/Trace Files/LatencyGraph.xlsx
+++ b/Experiment 1/Trace Files/LatencyGraph.xlsx
@@ -241,34 +241,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20.928355412799998</c:v>
+                  <c:v>65.378132476900007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.928226950300001</c:v>
+                  <c:v>65.377361702100004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.927335340599999</c:v>
+                  <c:v>65.372012043400005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.932727418700001</c:v>
+                  <c:v>65.404364512200004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.948023016200001</c:v>
+                  <c:v>65.496138097100001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.957212852000001</c:v>
+                  <c:v>65.550685905500004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.014766589299999</c:v>
+                  <c:v>65.892020270299994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.120052334</c:v>
+                  <c:v>72.517706666699993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.894913874699999</c:v>
+                  <c:v>71.169846681899998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23.3084147157</c:v>
+                  <c:v>79.074042553200002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -347,34 +347,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20.928355412799998</c:v>
+                  <c:v>65.378132476900007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.928226950300001</c:v>
+                  <c:v>65.377361702100004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.927335340599999</c:v>
+                  <c:v>65.372012043400005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.932727418700001</c:v>
+                  <c:v>65.404364512200004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.948023016200001</c:v>
+                  <c:v>65.496138097100001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.9598500225</c:v>
+                  <c:v>65.566465765800004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.029710230300001</c:v>
+                  <c:v>65.981368373400002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.8806972366</c:v>
+                  <c:v>71.078984474899997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.9828509602</c:v>
+                  <c:v>71.701067103100002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23.2762754098</c:v>
+                  <c:v>79.159333333299998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -453,34 +453,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20.928355412799998</c:v>
+                  <c:v>65.378132476900007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.928226950300001</c:v>
+                  <c:v>65.377361702100004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.927335340599999</c:v>
+                  <c:v>65.372012043400005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.932727418700001</c:v>
+                  <c:v>65.404364512200004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.948023016200001</c:v>
+                  <c:v>65.496138097100001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.9512462623</c:v>
+                  <c:v>65.514874312299995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.0197427821</c:v>
+                  <c:v>65.921846743299994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.1609262785</c:v>
+                  <c:v>72.7691390552</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.9651539119</c:v>
+                  <c:v>71.567791237099996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23.291156199700001</c:v>
+                  <c:v>79.590141414100003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,34 +559,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20.885040916499999</c:v>
+                  <c:v>65.1182454992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.919912711399999</c:v>
+                  <c:v>65.327476268400005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.919632160399999</c:v>
+                  <c:v>65.325792962400001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.9207659574</c:v>
+                  <c:v>65.332595744700001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.927419602400001</c:v>
+                  <c:v>65.371566345800005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.964693304699999</c:v>
+                  <c:v>65.5843394929</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.046566669000001</c:v>
+                  <c:v>66.0864955901</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.8543193167</c:v>
+                  <c:v>76.925689502200001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.9140970222</c:v>
+                  <c:v>77.273437447500001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.254171428599999</c:v>
+                  <c:v>73.073777777800004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -602,11 +602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1025530432"/>
-        <c:axId val="1025544576"/>
+        <c:axId val="1889858608"/>
+        <c:axId val="1889859696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1025530432"/>
+        <c:axId val="1889858608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1025544576"/>
+        <c:crossAx val="1889859696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,10 +713,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1025544576"/>
+        <c:axId val="1889859696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="20.5"/>
+          <c:max val="80"/>
+          <c:min val="60"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -821,7 +822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1025530432"/>
+        <c:crossAx val="1889858608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1759,7 +1760,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
@@ -1786,16 +1787,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>20.928355412799998</v>
+        <v>65.378132476900007</v>
       </c>
       <c r="C2">
-        <v>20.928355412799998</v>
+        <v>65.378132476900007</v>
       </c>
       <c r="D2">
-        <v>20.928355412799998</v>
+        <v>65.378132476900007</v>
       </c>
       <c r="E2">
-        <v>20.885040916499999</v>
+        <v>65.1182454992</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1803,16 +1804,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>20.928226950300001</v>
+        <v>65.377361702100004</v>
       </c>
       <c r="C3">
-        <v>20.928226950300001</v>
+        <v>65.377361702100004</v>
       </c>
       <c r="D3">
-        <v>20.928226950300001</v>
+        <v>65.377361702100004</v>
       </c>
       <c r="E3">
-        <v>20.919912711399999</v>
+        <v>65.327476268400005</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1820,16 +1821,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>20.927335340599999</v>
+        <v>65.372012043400005</v>
       </c>
       <c r="C4">
-        <v>20.927335340599999</v>
+        <v>65.372012043400005</v>
       </c>
       <c r="D4">
-        <v>20.927335340599999</v>
+        <v>65.372012043400005</v>
       </c>
       <c r="E4">
-        <v>20.919632160399999</v>
+        <v>65.325792962400001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1837,16 +1838,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>20.932727418700001</v>
+        <v>65.404364512200004</v>
       </c>
       <c r="C5">
-        <v>20.932727418700001</v>
+        <v>65.404364512200004</v>
       </c>
       <c r="D5">
-        <v>20.932727418700001</v>
+        <v>65.404364512200004</v>
       </c>
       <c r="E5">
-        <v>20.9207659574</v>
+        <v>65.332595744700001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1854,16 +1855,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>20.948023016200001</v>
+        <v>65.496138097100001</v>
       </c>
       <c r="C6">
-        <v>20.948023016200001</v>
+        <v>65.496138097100001</v>
       </c>
       <c r="D6">
-        <v>20.948023016200001</v>
+        <v>65.496138097100001</v>
       </c>
       <c r="E6">
-        <v>20.927419602400001</v>
+        <v>65.371566345800005</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1871,16 +1872,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>20.957212852000001</v>
+        <v>65.550685905500004</v>
       </c>
       <c r="C7">
-        <v>20.9598500225</v>
+        <v>65.566465765800004</v>
       </c>
       <c r="D7">
-        <v>20.9512462623</v>
+        <v>65.514874312299995</v>
       </c>
       <c r="E7">
-        <v>20.964693304699999</v>
+        <v>65.5843394929</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1888,16 +1889,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>21.014766589299999</v>
+        <v>65.892020270299994</v>
       </c>
       <c r="C8">
-        <v>21.029710230300001</v>
+        <v>65.981368373400002</v>
       </c>
       <c r="D8">
-        <v>21.0197427821</v>
+        <v>65.921846743299994</v>
       </c>
       <c r="E8">
-        <v>21.046566669000001</v>
+        <v>66.0864955901</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1905,16 +1906,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>22.120052334</v>
+        <v>72.517706666699993</v>
       </c>
       <c r="C9">
-        <v>21.8806972366</v>
+        <v>71.078984474899997</v>
       </c>
       <c r="D9">
-        <v>22.1609262785</v>
+        <v>72.7691390552</v>
       </c>
       <c r="E9">
-        <v>22.8543193167</v>
+        <v>76.925689502200001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1922,16 +1923,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>21.894913874699999</v>
+        <v>71.169846681899998</v>
       </c>
       <c r="C10">
-        <v>21.9828509602</v>
+        <v>71.701067103100002</v>
       </c>
       <c r="D10">
-        <v>21.9651539119</v>
+        <v>71.567791237099996</v>
       </c>
       <c r="E10">
-        <v>22.9140970222</v>
+        <v>77.273437447500001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1939,16 +1940,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>23.3084147157</v>
+        <v>79.074042553200002</v>
       </c>
       <c r="C11">
-        <v>23.2762754098</v>
+        <v>79.159333333299998</v>
       </c>
       <c r="D11">
-        <v>23.291156199700001</v>
+        <v>79.590141414100003</v>
       </c>
       <c r="E11">
-        <v>22.254171428599999</v>
+        <v>73.073777777800004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>